<commit_message>
Correction. Objective function ESSO subproblem (mistakenly modified in previous commit!)
</commit_message>
<xml_diff>
--- a/data/CS1_4/case30/case30_base.xlsx
+++ b/data/CS1_4/case30/case30_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\CS1_4\case30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D09EA6A-66C0-4C1A-B776-DB68B9B50585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA187050-851E-4E62-9E1D-D05880241510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28410" yWindow="555" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="450" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="34" r:id="rId1"/>
@@ -736,7 +736,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>